<commit_message>
Added departmentSimple column to HR records with proper database schema migration
</commit_message>
<xml_diff>
--- a/FLC/Templates/HR_template.xlsx
+++ b/FLC/Templates/HR_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mirko/Library/Mobile Documents/com~apple~CloudDocs/ONTWIKKEL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C66524EB-C95A-0145-B645-42658EBB7ACA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F732B845-033A-A940-BF78-D52D66F6FB20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2680" yWindow="1620" windowWidth="38680" windowHeight="18980" xr2:uid="{5B1D9164-7E89-F143-8CBA-963F7DE74F5E}"/>
   </bookViews>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
   <si>
     <t>System Account</t>
   </si>
@@ -86,9 +86,6 @@
     <t>Leave Date</t>
   </si>
   <si>
-    <t>Employee Number</t>
-  </si>
-  <si>
     <t>HR Data Collection Template</t>
   </si>
   <si>
@@ -122,9 +119,6 @@
     <t>Date (DD-MM-YYYY)</t>
   </si>
   <si>
-    <t>Text (7 digits)</t>
-  </si>
-  <si>
     <t>jdoe</t>
   </si>
   <si>
@@ -140,7 +134,10 @@
     <t>'=== START DATA BELOW ==='</t>
   </si>
   <si>
-    <t>Employee number</t>
+    <t>Tekst</t>
+  </si>
+  <si>
+    <t>Departement Simple</t>
   </si>
 </sst>
 </file>
@@ -199,11 +196,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="hr_test_data" connectionId="1" xr16:uid="{676159C6-668A-784A-97F0-A98EA83D1DBD}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="hr_test_data_1" connectionId="2" xr16:uid="{31924EC3-DF8A-5A4D-A186-2FF7588D569D}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="hr_test_data" connectionId="1" xr16:uid="{676159C6-668A-784A-97F0-A98EA83D1DBD}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -526,7 +523,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD33"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -536,47 +533,47 @@
     <col min="3" max="3" width="32.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="2"/>
@@ -598,48 +595,46 @@
         <v>4</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
         <v>12</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>13</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>14</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="F8" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
         <v>18</v>
       </c>
-      <c r="B9" t="s">
+      <c r="D9" t="s">
         <v>19</v>
-      </c>
-      <c r="C9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" t="s">
-        <v>21</v>
       </c>
       <c r="E9" s="1">
         <v>45657</v>
       </c>
-      <c r="F9" s="2">
-        <v>1234567</v>
-      </c>
+      <c r="F9" s="2"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E10" s="1"/>
@@ -647,7 +642,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="2"/>
@@ -668,8 +663,8 @@
       <c r="E13" t="s">
         <v>4</v>
       </c>
-      <c r="F13" t="s">
-        <v>5</v>
+      <c r="F13" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="5:5" x14ac:dyDescent="0.2">

</xml_diff>